<commit_message>
Primera versión de mapeo mediante r2rml
- todavia no esta completo
- las IRI de algunos elementos aún no están bien generadas
</commit_message>
<xml_diff>
--- a/data_mappeator/InputPhotocalysisMapping.xlsx
+++ b/data_mappeator/InputPhotocalysisMapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="150">
   <si>
     <t xml:space="preserve">Prefix</t>
   </si>
@@ -128,7 +128,7 @@
     <t xml:space="preserve">schema:Person</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.example.com/author/{AUTHOR_NAME}-{ID}</t>
+    <t xml:space="preserve">http://data.example.com/author/{NAME}-{ID}</t>
   </si>
   <si>
     <t xml:space="preserve">MaterialTransformationProcess</t>
@@ -203,6 +203,33 @@
     <t xml:space="preserve">http://data.example.com/output_quantity/{ID}-{UNIT}</t>
   </si>
   <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://en.wikipedia.org/wiki/{COUNTRY_NAME}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qudt:Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit:{UNIT}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaterialTransformationRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:MaterialTransformationRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.example.com/material_transformation_role/{Role}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feature</t>
   </si>
   <si>
@@ -234,6 +261,9 @@
   </si>
   <si>
     <t xml:space="preserve">chemicals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">units</t>
   </si>
   <si>
     <t xml:space="preserve">Predicate</t>
@@ -383,22 +413,16 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">{PAPER_ID}</t>
+    <t xml:space="preserve">{PAPERID}</t>
   </si>
   <si>
     <t xml:space="preserve">schema:name</t>
   </si>
   <si>
-    <t xml:space="preserve">{AUTHOR_NAME}</t>
-  </si>
-  <si>
     <t xml:space="preserve">phcat:affiliationCountry</t>
   </si>
   <si>
-    <t xml:space="preserve">https://en.wikipedia.org/wiki/{country_name}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:Country</t>
+    <t xml:space="preserve">{COUNTRY}</t>
   </si>
   <si>
     <t xml:space="preserve">phcat:reportedIn</t>
@@ -431,6 +455,9 @@
     <t xml:space="preserve">phcat:hasCondition</t>
   </si>
   <si>
+    <t xml:space="preserve">phcat:hasOutput</t>
+  </si>
+  <si>
     <t xml:space="preserve">qudt:numericValue</t>
   </si>
   <si>
@@ -446,9 +473,6 @@
     <t xml:space="preserve">unit:EV</t>
   </si>
   <si>
-    <t xml:space="preserve">qudt:Unit</t>
-  </si>
-  <si>
     <t xml:space="preserve">{BET_M2_G}</t>
   </si>
   <si>
@@ -479,10 +503,7 @@
     <t xml:space="preserve">phcat:hasRole</t>
   </si>
   <si>
-    <t xml:space="preserve">phcat:{ROLE}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phcat:MaterialTransformationRole</t>
+    <t xml:space="preserve">{ROLE}</t>
   </si>
   <si>
     <t xml:space="preserve">phcat:conditionType</t>
@@ -497,16 +518,16 @@
     <t xml:space="preserve">{QUANTITY}</t>
   </si>
   <si>
-    <t xml:space="preserve">unit:{UNIT}</t>
+    <t xml:space="preserve">{QUDT_UNIT}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{UNIT}</t>
   </si>
   <si>
     <t xml:space="preserve">phcat:hasOutputCuantity</t>
   </si>
   <si>
     <t xml:space="preserve">phcat:numericValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unit:{QUDT_UNIT}</t>
   </si>
   <si>
     <t xml:space="preserve">FunctionID</t>
@@ -681,6 +702,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -691,10 +716,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1932,7 +1953,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2077,12 +2098,44 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C18" s="11"/>
+    </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3067,11 +3120,13 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" display="http://data.example.com/input/{ID}"/>
-    <hyperlink ref="C7" r:id="rId2" display="http://data.example.com/condition/{ID}"/>
-    <hyperlink ref="C8" r:id="rId3" display="http://data.example.com/output/{ID}"/>
-    <hyperlink ref="C9" r:id="rId4" display="http://data.example.com/eg/{ID}"/>
-    <hyperlink ref="C10" r:id="rId5" display="http://data.example.com/bet/{ID}"/>
+    <hyperlink ref="C4" r:id="rId1" display="http://data.example.com/author/"/>
+    <hyperlink ref="C6" r:id="rId2" display="http://data.example.com/input/{ID}"/>
+    <hyperlink ref="C7" r:id="rId3" display="http://data.example.com/condition/{ID}"/>
+    <hyperlink ref="C8" r:id="rId4" display="http://data.example.com/output/{ID}"/>
+    <hyperlink ref="C9" r:id="rId5" display="http://data.example.com/eg/{ID}"/>
+    <hyperlink ref="C10" r:id="rId6" display="http://data.example.com/bet/{ID}"/>
+    <hyperlink ref="C13" r:id="rId7" display="https://en.wikipedia.org/wiki/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3088,10 +3143,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C992"/>
+  <dimension ref="A1:AMJ993"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3105,14 +3160,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>60</v>
+      <c r="B1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3120,10 +3175,10 @@
         <v>26</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3131,114 +3186,1165 @@
         <v>29</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="B6" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
+      <c r="N14" s="0"/>
+      <c r="O14" s="0"/>
+      <c r="P14" s="0"/>
+      <c r="Q14" s="0"/>
+      <c r="R14" s="0"/>
+      <c r="S14" s="0"/>
+      <c r="T14" s="0"/>
+      <c r="U14" s="0"/>
+      <c r="V14" s="0"/>
+      <c r="W14" s="0"/>
+      <c r="X14" s="0"/>
+      <c r="Y14" s="0"/>
+      <c r="Z14" s="0"/>
+      <c r="AA14" s="0"/>
+      <c r="AB14" s="0"/>
+      <c r="AC14" s="0"/>
+      <c r="AD14" s="0"/>
+      <c r="AE14" s="0"/>
+      <c r="AF14" s="0"/>
+      <c r="AG14" s="0"/>
+      <c r="AH14" s="0"/>
+      <c r="AI14" s="0"/>
+      <c r="AJ14" s="0"/>
+      <c r="AK14" s="0"/>
+      <c r="AL14" s="0"/>
+      <c r="AM14" s="0"/>
+      <c r="AN14" s="0"/>
+      <c r="AO14" s="0"/>
+      <c r="AP14" s="0"/>
+      <c r="AQ14" s="0"/>
+      <c r="AR14" s="0"/>
+      <c r="AS14" s="0"/>
+      <c r="AT14" s="0"/>
+      <c r="AU14" s="0"/>
+      <c r="AV14" s="0"/>
+      <c r="AW14" s="0"/>
+      <c r="AX14" s="0"/>
+      <c r="AY14" s="0"/>
+      <c r="AZ14" s="0"/>
+      <c r="BA14" s="0"/>
+      <c r="BB14" s="0"/>
+      <c r="BC14" s="0"/>
+      <c r="BD14" s="0"/>
+      <c r="BE14" s="0"/>
+      <c r="BF14" s="0"/>
+      <c r="BG14" s="0"/>
+      <c r="BH14" s="0"/>
+      <c r="BI14" s="0"/>
+      <c r="BJ14" s="0"/>
+      <c r="BK14" s="0"/>
+      <c r="BL14" s="0"/>
+      <c r="BM14" s="0"/>
+      <c r="BN14" s="0"/>
+      <c r="BO14" s="0"/>
+      <c r="BP14" s="0"/>
+      <c r="BQ14" s="0"/>
+      <c r="BR14" s="0"/>
+      <c r="BS14" s="0"/>
+      <c r="BT14" s="0"/>
+      <c r="BU14" s="0"/>
+      <c r="BV14" s="0"/>
+      <c r="BW14" s="0"/>
+      <c r="BX14" s="0"/>
+      <c r="BY14" s="0"/>
+      <c r="BZ14" s="0"/>
+      <c r="CA14" s="0"/>
+      <c r="CB14" s="0"/>
+      <c r="CC14" s="0"/>
+      <c r="CD14" s="0"/>
+      <c r="CE14" s="0"/>
+      <c r="CF14" s="0"/>
+      <c r="CG14" s="0"/>
+      <c r="CH14" s="0"/>
+      <c r="CI14" s="0"/>
+      <c r="CJ14" s="0"/>
+      <c r="CK14" s="0"/>
+      <c r="CL14" s="0"/>
+      <c r="CM14" s="0"/>
+      <c r="CN14" s="0"/>
+      <c r="CO14" s="0"/>
+      <c r="CP14" s="0"/>
+      <c r="CQ14" s="0"/>
+      <c r="CR14" s="0"/>
+      <c r="CS14" s="0"/>
+      <c r="CT14" s="0"/>
+      <c r="CU14" s="0"/>
+      <c r="CV14" s="0"/>
+      <c r="CW14" s="0"/>
+      <c r="CX14" s="0"/>
+      <c r="CY14" s="0"/>
+      <c r="CZ14" s="0"/>
+      <c r="DA14" s="0"/>
+      <c r="DB14" s="0"/>
+      <c r="DC14" s="0"/>
+      <c r="DD14" s="0"/>
+      <c r="DE14" s="0"/>
+      <c r="DF14" s="0"/>
+      <c r="DG14" s="0"/>
+      <c r="DH14" s="0"/>
+      <c r="DI14" s="0"/>
+      <c r="DJ14" s="0"/>
+      <c r="DK14" s="0"/>
+      <c r="DL14" s="0"/>
+      <c r="DM14" s="0"/>
+      <c r="DN14" s="0"/>
+      <c r="DO14" s="0"/>
+      <c r="DP14" s="0"/>
+      <c r="DQ14" s="0"/>
+      <c r="DR14" s="0"/>
+      <c r="DS14" s="0"/>
+      <c r="DT14" s="0"/>
+      <c r="DU14" s="0"/>
+      <c r="DV14" s="0"/>
+      <c r="DW14" s="0"/>
+      <c r="DX14" s="0"/>
+      <c r="DY14" s="0"/>
+      <c r="DZ14" s="0"/>
+      <c r="EA14" s="0"/>
+      <c r="EB14" s="0"/>
+      <c r="EC14" s="0"/>
+      <c r="ED14" s="0"/>
+      <c r="EE14" s="0"/>
+      <c r="EF14" s="0"/>
+      <c r="EG14" s="0"/>
+      <c r="EH14" s="0"/>
+      <c r="EI14" s="0"/>
+      <c r="EJ14" s="0"/>
+      <c r="EK14" s="0"/>
+      <c r="EL14" s="0"/>
+      <c r="EM14" s="0"/>
+      <c r="EN14" s="0"/>
+      <c r="EO14" s="0"/>
+      <c r="EP14" s="0"/>
+      <c r="EQ14" s="0"/>
+      <c r="ER14" s="0"/>
+      <c r="ES14" s="0"/>
+      <c r="ET14" s="0"/>
+      <c r="EU14" s="0"/>
+      <c r="EV14" s="0"/>
+      <c r="EW14" s="0"/>
+      <c r="EX14" s="0"/>
+      <c r="EY14" s="0"/>
+      <c r="EZ14" s="0"/>
+      <c r="FA14" s="0"/>
+      <c r="FB14" s="0"/>
+      <c r="FC14" s="0"/>
+      <c r="FD14" s="0"/>
+      <c r="FE14" s="0"/>
+      <c r="FF14" s="0"/>
+      <c r="FG14" s="0"/>
+      <c r="FH14" s="0"/>
+      <c r="FI14" s="0"/>
+      <c r="FJ14" s="0"/>
+      <c r="FK14" s="0"/>
+      <c r="FL14" s="0"/>
+      <c r="FM14" s="0"/>
+      <c r="FN14" s="0"/>
+      <c r="FO14" s="0"/>
+      <c r="FP14" s="0"/>
+      <c r="FQ14" s="0"/>
+      <c r="FR14" s="0"/>
+      <c r="FS14" s="0"/>
+      <c r="FT14" s="0"/>
+      <c r="FU14" s="0"/>
+      <c r="FV14" s="0"/>
+      <c r="FW14" s="0"/>
+      <c r="FX14" s="0"/>
+      <c r="FY14" s="0"/>
+      <c r="FZ14" s="0"/>
+      <c r="GA14" s="0"/>
+      <c r="GB14" s="0"/>
+      <c r="GC14" s="0"/>
+      <c r="GD14" s="0"/>
+      <c r="GE14" s="0"/>
+      <c r="GF14" s="0"/>
+      <c r="GG14" s="0"/>
+      <c r="GH14" s="0"/>
+      <c r="GI14" s="0"/>
+      <c r="GJ14" s="0"/>
+      <c r="GK14" s="0"/>
+      <c r="GL14" s="0"/>
+      <c r="GM14" s="0"/>
+      <c r="GN14" s="0"/>
+      <c r="GO14" s="0"/>
+      <c r="GP14" s="0"/>
+      <c r="GQ14" s="0"/>
+      <c r="GR14" s="0"/>
+      <c r="GS14" s="0"/>
+      <c r="GT14" s="0"/>
+      <c r="GU14" s="0"/>
+      <c r="GV14" s="0"/>
+      <c r="GW14" s="0"/>
+      <c r="GX14" s="0"/>
+      <c r="GY14" s="0"/>
+      <c r="GZ14" s="0"/>
+      <c r="HA14" s="0"/>
+      <c r="HB14" s="0"/>
+      <c r="HC14" s="0"/>
+      <c r="HD14" s="0"/>
+      <c r="HE14" s="0"/>
+      <c r="HF14" s="0"/>
+      <c r="HG14" s="0"/>
+      <c r="HH14" s="0"/>
+      <c r="HI14" s="0"/>
+      <c r="HJ14" s="0"/>
+      <c r="HK14" s="0"/>
+      <c r="HL14" s="0"/>
+      <c r="HM14" s="0"/>
+      <c r="HN14" s="0"/>
+      <c r="HO14" s="0"/>
+      <c r="HP14" s="0"/>
+      <c r="HQ14" s="0"/>
+      <c r="HR14" s="0"/>
+      <c r="HS14" s="0"/>
+      <c r="HT14" s="0"/>
+      <c r="HU14" s="0"/>
+      <c r="HV14" s="0"/>
+      <c r="HW14" s="0"/>
+      <c r="HX14" s="0"/>
+      <c r="HY14" s="0"/>
+      <c r="HZ14" s="0"/>
+      <c r="IA14" s="0"/>
+      <c r="IB14" s="0"/>
+      <c r="IC14" s="0"/>
+      <c r="ID14" s="0"/>
+      <c r="IE14" s="0"/>
+      <c r="IF14" s="0"/>
+      <c r="IG14" s="0"/>
+      <c r="IH14" s="0"/>
+      <c r="II14" s="0"/>
+      <c r="IJ14" s="0"/>
+      <c r="IK14" s="0"/>
+      <c r="IL14" s="0"/>
+      <c r="IM14" s="0"/>
+      <c r="IN14" s="0"/>
+      <c r="IO14" s="0"/>
+      <c r="IP14" s="0"/>
+      <c r="IQ14" s="0"/>
+      <c r="IR14" s="0"/>
+      <c r="IS14" s="0"/>
+      <c r="IT14" s="0"/>
+      <c r="IU14" s="0"/>
+      <c r="IV14" s="0"/>
+      <c r="IW14" s="0"/>
+      <c r="IX14" s="0"/>
+      <c r="IY14" s="0"/>
+      <c r="IZ14" s="0"/>
+      <c r="JA14" s="0"/>
+      <c r="JB14" s="0"/>
+      <c r="JC14" s="0"/>
+      <c r="JD14" s="0"/>
+      <c r="JE14" s="0"/>
+      <c r="JF14" s="0"/>
+      <c r="JG14" s="0"/>
+      <c r="JH14" s="0"/>
+      <c r="JI14" s="0"/>
+      <c r="JJ14" s="0"/>
+      <c r="JK14" s="0"/>
+      <c r="JL14" s="0"/>
+      <c r="JM14" s="0"/>
+      <c r="JN14" s="0"/>
+      <c r="JO14" s="0"/>
+      <c r="JP14" s="0"/>
+      <c r="JQ14" s="0"/>
+      <c r="JR14" s="0"/>
+      <c r="JS14" s="0"/>
+      <c r="JT14" s="0"/>
+      <c r="JU14" s="0"/>
+      <c r="JV14" s="0"/>
+      <c r="JW14" s="0"/>
+      <c r="JX14" s="0"/>
+      <c r="JY14" s="0"/>
+      <c r="JZ14" s="0"/>
+      <c r="KA14" s="0"/>
+      <c r="KB14" s="0"/>
+      <c r="KC14" s="0"/>
+      <c r="KD14" s="0"/>
+      <c r="KE14" s="0"/>
+      <c r="KF14" s="0"/>
+      <c r="KG14" s="0"/>
+      <c r="KH14" s="0"/>
+      <c r="KI14" s="0"/>
+      <c r="KJ14" s="0"/>
+      <c r="KK14" s="0"/>
+      <c r="KL14" s="0"/>
+      <c r="KM14" s="0"/>
+      <c r="KN14" s="0"/>
+      <c r="KO14" s="0"/>
+      <c r="KP14" s="0"/>
+      <c r="KQ14" s="0"/>
+      <c r="KR14" s="0"/>
+      <c r="KS14" s="0"/>
+      <c r="KT14" s="0"/>
+      <c r="KU14" s="0"/>
+      <c r="KV14" s="0"/>
+      <c r="KW14" s="0"/>
+      <c r="KX14" s="0"/>
+      <c r="KY14" s="0"/>
+      <c r="KZ14" s="0"/>
+      <c r="LA14" s="0"/>
+      <c r="LB14" s="0"/>
+      <c r="LC14" s="0"/>
+      <c r="LD14" s="0"/>
+      <c r="LE14" s="0"/>
+      <c r="LF14" s="0"/>
+      <c r="LG14" s="0"/>
+      <c r="LH14" s="0"/>
+      <c r="LI14" s="0"/>
+      <c r="LJ14" s="0"/>
+      <c r="LK14" s="0"/>
+      <c r="LL14" s="0"/>
+      <c r="LM14" s="0"/>
+      <c r="LN14" s="0"/>
+      <c r="LO14" s="0"/>
+      <c r="LP14" s="0"/>
+      <c r="LQ14" s="0"/>
+      <c r="LR14" s="0"/>
+      <c r="LS14" s="0"/>
+      <c r="LT14" s="0"/>
+      <c r="LU14" s="0"/>
+      <c r="LV14" s="0"/>
+      <c r="LW14" s="0"/>
+      <c r="LX14" s="0"/>
+      <c r="LY14" s="0"/>
+      <c r="LZ14" s="0"/>
+      <c r="MA14" s="0"/>
+      <c r="MB14" s="0"/>
+      <c r="MC14" s="0"/>
+      <c r="MD14" s="0"/>
+      <c r="ME14" s="0"/>
+      <c r="MF14" s="0"/>
+      <c r="MG14" s="0"/>
+      <c r="MH14" s="0"/>
+      <c r="MI14" s="0"/>
+      <c r="MJ14" s="0"/>
+      <c r="MK14" s="0"/>
+      <c r="ML14" s="0"/>
+      <c r="MM14" s="0"/>
+      <c r="MN14" s="0"/>
+      <c r="MO14" s="0"/>
+      <c r="MP14" s="0"/>
+      <c r="MQ14" s="0"/>
+      <c r="MR14" s="0"/>
+      <c r="MS14" s="0"/>
+      <c r="MT14" s="0"/>
+      <c r="MU14" s="0"/>
+      <c r="MV14" s="0"/>
+      <c r="MW14" s="0"/>
+      <c r="MX14" s="0"/>
+      <c r="MY14" s="0"/>
+      <c r="MZ14" s="0"/>
+      <c r="NA14" s="0"/>
+      <c r="NB14" s="0"/>
+      <c r="NC14" s="0"/>
+      <c r="ND14" s="0"/>
+      <c r="NE14" s="0"/>
+      <c r="NF14" s="0"/>
+      <c r="NG14" s="0"/>
+      <c r="NH14" s="0"/>
+      <c r="NI14" s="0"/>
+      <c r="NJ14" s="0"/>
+      <c r="NK14" s="0"/>
+      <c r="NL14" s="0"/>
+      <c r="NM14" s="0"/>
+      <c r="NN14" s="0"/>
+      <c r="NO14" s="0"/>
+      <c r="NP14" s="0"/>
+      <c r="NQ14" s="0"/>
+      <c r="NR14" s="0"/>
+      <c r="NS14" s="0"/>
+      <c r="NT14" s="0"/>
+      <c r="NU14" s="0"/>
+      <c r="NV14" s="0"/>
+      <c r="NW14" s="0"/>
+      <c r="NX14" s="0"/>
+      <c r="NY14" s="0"/>
+      <c r="NZ14" s="0"/>
+      <c r="OA14" s="0"/>
+      <c r="OB14" s="0"/>
+      <c r="OC14" s="0"/>
+      <c r="OD14" s="0"/>
+      <c r="OE14" s="0"/>
+      <c r="OF14" s="0"/>
+      <c r="OG14" s="0"/>
+      <c r="OH14" s="0"/>
+      <c r="OI14" s="0"/>
+      <c r="OJ14" s="0"/>
+      <c r="OK14" s="0"/>
+      <c r="OL14" s="0"/>
+      <c r="OM14" s="0"/>
+      <c r="ON14" s="0"/>
+      <c r="OO14" s="0"/>
+      <c r="OP14" s="0"/>
+      <c r="OQ14" s="0"/>
+      <c r="OR14" s="0"/>
+      <c r="OS14" s="0"/>
+      <c r="OT14" s="0"/>
+      <c r="OU14" s="0"/>
+      <c r="OV14" s="0"/>
+      <c r="OW14" s="0"/>
+      <c r="OX14" s="0"/>
+      <c r="OY14" s="0"/>
+      <c r="OZ14" s="0"/>
+      <c r="PA14" s="0"/>
+      <c r="PB14" s="0"/>
+      <c r="PC14" s="0"/>
+      <c r="PD14" s="0"/>
+      <c r="PE14" s="0"/>
+      <c r="PF14" s="0"/>
+      <c r="PG14" s="0"/>
+      <c r="PH14" s="0"/>
+      <c r="PI14" s="0"/>
+      <c r="PJ14" s="0"/>
+      <c r="PK14" s="0"/>
+      <c r="PL14" s="0"/>
+      <c r="PM14" s="0"/>
+      <c r="PN14" s="0"/>
+      <c r="PO14" s="0"/>
+      <c r="PP14" s="0"/>
+      <c r="PQ14" s="0"/>
+      <c r="PR14" s="0"/>
+      <c r="PS14" s="0"/>
+      <c r="PT14" s="0"/>
+      <c r="PU14" s="0"/>
+      <c r="PV14" s="0"/>
+      <c r="PW14" s="0"/>
+      <c r="PX14" s="0"/>
+      <c r="PY14" s="0"/>
+      <c r="PZ14" s="0"/>
+      <c r="QA14" s="0"/>
+      <c r="QB14" s="0"/>
+      <c r="QC14" s="0"/>
+      <c r="QD14" s="0"/>
+      <c r="QE14" s="0"/>
+      <c r="QF14" s="0"/>
+      <c r="QG14" s="0"/>
+      <c r="QH14" s="0"/>
+      <c r="QI14" s="0"/>
+      <c r="QJ14" s="0"/>
+      <c r="QK14" s="0"/>
+      <c r="QL14" s="0"/>
+      <c r="QM14" s="0"/>
+      <c r="QN14" s="0"/>
+      <c r="QO14" s="0"/>
+      <c r="QP14" s="0"/>
+      <c r="QQ14" s="0"/>
+      <c r="QR14" s="0"/>
+      <c r="QS14" s="0"/>
+      <c r="QT14" s="0"/>
+      <c r="QU14" s="0"/>
+      <c r="QV14" s="0"/>
+      <c r="QW14" s="0"/>
+      <c r="QX14" s="0"/>
+      <c r="QY14" s="0"/>
+      <c r="QZ14" s="0"/>
+      <c r="RA14" s="0"/>
+      <c r="RB14" s="0"/>
+      <c r="RC14" s="0"/>
+      <c r="RD14" s="0"/>
+      <c r="RE14" s="0"/>
+      <c r="RF14" s="0"/>
+      <c r="RG14" s="0"/>
+      <c r="RH14" s="0"/>
+      <c r="RI14" s="0"/>
+      <c r="RJ14" s="0"/>
+      <c r="RK14" s="0"/>
+      <c r="RL14" s="0"/>
+      <c r="RM14" s="0"/>
+      <c r="RN14" s="0"/>
+      <c r="RO14" s="0"/>
+      <c r="RP14" s="0"/>
+      <c r="RQ14" s="0"/>
+      <c r="RR14" s="0"/>
+      <c r="RS14" s="0"/>
+      <c r="RT14" s="0"/>
+      <c r="RU14" s="0"/>
+      <c r="RV14" s="0"/>
+      <c r="RW14" s="0"/>
+      <c r="RX14" s="0"/>
+      <c r="RY14" s="0"/>
+      <c r="RZ14" s="0"/>
+      <c r="SA14" s="0"/>
+      <c r="SB14" s="0"/>
+      <c r="SC14" s="0"/>
+      <c r="SD14" s="0"/>
+      <c r="SE14" s="0"/>
+      <c r="SF14" s="0"/>
+      <c r="SG14" s="0"/>
+      <c r="SH14" s="0"/>
+      <c r="SI14" s="0"/>
+      <c r="SJ14" s="0"/>
+      <c r="SK14" s="0"/>
+      <c r="SL14" s="0"/>
+      <c r="SM14" s="0"/>
+      <c r="SN14" s="0"/>
+      <c r="SO14" s="0"/>
+      <c r="SP14" s="0"/>
+      <c r="SQ14" s="0"/>
+      <c r="SR14" s="0"/>
+      <c r="SS14" s="0"/>
+      <c r="ST14" s="0"/>
+      <c r="SU14" s="0"/>
+      <c r="SV14" s="0"/>
+      <c r="SW14" s="0"/>
+      <c r="SX14" s="0"/>
+      <c r="SY14" s="0"/>
+      <c r="SZ14" s="0"/>
+      <c r="TA14" s="0"/>
+      <c r="TB14" s="0"/>
+      <c r="TC14" s="0"/>
+      <c r="TD14" s="0"/>
+      <c r="TE14" s="0"/>
+      <c r="TF14" s="0"/>
+      <c r="TG14" s="0"/>
+      <c r="TH14" s="0"/>
+      <c r="TI14" s="0"/>
+      <c r="TJ14" s="0"/>
+      <c r="TK14" s="0"/>
+      <c r="TL14" s="0"/>
+      <c r="TM14" s="0"/>
+      <c r="TN14" s="0"/>
+      <c r="TO14" s="0"/>
+      <c r="TP14" s="0"/>
+      <c r="TQ14" s="0"/>
+      <c r="TR14" s="0"/>
+      <c r="TS14" s="0"/>
+      <c r="TT14" s="0"/>
+      <c r="TU14" s="0"/>
+      <c r="TV14" s="0"/>
+      <c r="TW14" s="0"/>
+      <c r="TX14" s="0"/>
+      <c r="TY14" s="0"/>
+      <c r="TZ14" s="0"/>
+      <c r="UA14" s="0"/>
+      <c r="UB14" s="0"/>
+      <c r="UC14" s="0"/>
+      <c r="UD14" s="0"/>
+      <c r="UE14" s="0"/>
+      <c r="UF14" s="0"/>
+      <c r="UG14" s="0"/>
+      <c r="UH14" s="0"/>
+      <c r="UI14" s="0"/>
+      <c r="UJ14" s="0"/>
+      <c r="UK14" s="0"/>
+      <c r="UL14" s="0"/>
+      <c r="UM14" s="0"/>
+      <c r="UN14" s="0"/>
+      <c r="UO14" s="0"/>
+      <c r="UP14" s="0"/>
+      <c r="UQ14" s="0"/>
+      <c r="UR14" s="0"/>
+      <c r="US14" s="0"/>
+      <c r="UT14" s="0"/>
+      <c r="UU14" s="0"/>
+      <c r="UV14" s="0"/>
+      <c r="UW14" s="0"/>
+      <c r="UX14" s="0"/>
+      <c r="UY14" s="0"/>
+      <c r="UZ14" s="0"/>
+      <c r="VA14" s="0"/>
+      <c r="VB14" s="0"/>
+      <c r="VC14" s="0"/>
+      <c r="VD14" s="0"/>
+      <c r="VE14" s="0"/>
+      <c r="VF14" s="0"/>
+      <c r="VG14" s="0"/>
+      <c r="VH14" s="0"/>
+      <c r="VI14" s="0"/>
+      <c r="VJ14" s="0"/>
+      <c r="VK14" s="0"/>
+      <c r="VL14" s="0"/>
+      <c r="VM14" s="0"/>
+      <c r="VN14" s="0"/>
+      <c r="VO14" s="0"/>
+      <c r="VP14" s="0"/>
+      <c r="VQ14" s="0"/>
+      <c r="VR14" s="0"/>
+      <c r="VS14" s="0"/>
+      <c r="VT14" s="0"/>
+      <c r="VU14" s="0"/>
+      <c r="VV14" s="0"/>
+      <c r="VW14" s="0"/>
+      <c r="VX14" s="0"/>
+      <c r="VY14" s="0"/>
+      <c r="VZ14" s="0"/>
+      <c r="WA14" s="0"/>
+      <c r="WB14" s="0"/>
+      <c r="WC14" s="0"/>
+      <c r="WD14" s="0"/>
+      <c r="WE14" s="0"/>
+      <c r="WF14" s="0"/>
+      <c r="WG14" s="0"/>
+      <c r="WH14" s="0"/>
+      <c r="WI14" s="0"/>
+      <c r="WJ14" s="0"/>
+      <c r="WK14" s="0"/>
+      <c r="WL14" s="0"/>
+      <c r="WM14" s="0"/>
+      <c r="WN14" s="0"/>
+      <c r="WO14" s="0"/>
+      <c r="WP14" s="0"/>
+      <c r="WQ14" s="0"/>
+      <c r="WR14" s="0"/>
+      <c r="WS14" s="0"/>
+      <c r="WT14" s="0"/>
+      <c r="WU14" s="0"/>
+      <c r="WV14" s="0"/>
+      <c r="WW14" s="0"/>
+      <c r="WX14" s="0"/>
+      <c r="WY14" s="0"/>
+      <c r="WZ14" s="0"/>
+      <c r="XA14" s="0"/>
+      <c r="XB14" s="0"/>
+      <c r="XC14" s="0"/>
+      <c r="XD14" s="0"/>
+      <c r="XE14" s="0"/>
+      <c r="XF14" s="0"/>
+      <c r="XG14" s="0"/>
+      <c r="XH14" s="0"/>
+      <c r="XI14" s="0"/>
+      <c r="XJ14" s="0"/>
+      <c r="XK14" s="0"/>
+      <c r="XL14" s="0"/>
+      <c r="XM14" s="0"/>
+      <c r="XN14" s="0"/>
+      <c r="XO14" s="0"/>
+      <c r="XP14" s="0"/>
+      <c r="XQ14" s="0"/>
+      <c r="XR14" s="0"/>
+      <c r="XS14" s="0"/>
+      <c r="XT14" s="0"/>
+      <c r="XU14" s="0"/>
+      <c r="XV14" s="0"/>
+      <c r="XW14" s="0"/>
+      <c r="XX14" s="0"/>
+      <c r="XY14" s="0"/>
+      <c r="XZ14" s="0"/>
+      <c r="YA14" s="0"/>
+      <c r="YB14" s="0"/>
+      <c r="YC14" s="0"/>
+      <c r="YD14" s="0"/>
+      <c r="YE14" s="0"/>
+      <c r="YF14" s="0"/>
+      <c r="YG14" s="0"/>
+      <c r="YH14" s="0"/>
+      <c r="YI14" s="0"/>
+      <c r="YJ14" s="0"/>
+      <c r="YK14" s="0"/>
+      <c r="YL14" s="0"/>
+      <c r="YM14" s="0"/>
+      <c r="YN14" s="0"/>
+      <c r="YO14" s="0"/>
+      <c r="YP14" s="0"/>
+      <c r="YQ14" s="0"/>
+      <c r="YR14" s="0"/>
+      <c r="YS14" s="0"/>
+      <c r="YT14" s="0"/>
+      <c r="YU14" s="0"/>
+      <c r="YV14" s="0"/>
+      <c r="YW14" s="0"/>
+      <c r="YX14" s="0"/>
+      <c r="YY14" s="0"/>
+      <c r="YZ14" s="0"/>
+      <c r="ZA14" s="0"/>
+      <c r="ZB14" s="0"/>
+      <c r="ZC14" s="0"/>
+      <c r="ZD14" s="0"/>
+      <c r="ZE14" s="0"/>
+      <c r="ZF14" s="0"/>
+      <c r="ZG14" s="0"/>
+      <c r="ZH14" s="0"/>
+      <c r="ZI14" s="0"/>
+      <c r="ZJ14" s="0"/>
+      <c r="ZK14" s="0"/>
+      <c r="ZL14" s="0"/>
+      <c r="ZM14" s="0"/>
+      <c r="ZN14" s="0"/>
+      <c r="ZO14" s="0"/>
+      <c r="ZP14" s="0"/>
+      <c r="ZQ14" s="0"/>
+      <c r="ZR14" s="0"/>
+      <c r="ZS14" s="0"/>
+      <c r="ZT14" s="0"/>
+      <c r="ZU14" s="0"/>
+      <c r="ZV14" s="0"/>
+      <c r="ZW14" s="0"/>
+      <c r="ZX14" s="0"/>
+      <c r="ZY14" s="0"/>
+      <c r="ZZ14" s="0"/>
+      <c r="AAA14" s="0"/>
+      <c r="AAB14" s="0"/>
+      <c r="AAC14" s="0"/>
+      <c r="AAD14" s="0"/>
+      <c r="AAE14" s="0"/>
+      <c r="AAF14" s="0"/>
+      <c r="AAG14" s="0"/>
+      <c r="AAH14" s="0"/>
+      <c r="AAI14" s="0"/>
+      <c r="AAJ14" s="0"/>
+      <c r="AAK14" s="0"/>
+      <c r="AAL14" s="0"/>
+      <c r="AAM14" s="0"/>
+      <c r="AAN14" s="0"/>
+      <c r="AAO14" s="0"/>
+      <c r="AAP14" s="0"/>
+      <c r="AAQ14" s="0"/>
+      <c r="AAR14" s="0"/>
+      <c r="AAS14" s="0"/>
+      <c r="AAT14" s="0"/>
+      <c r="AAU14" s="0"/>
+      <c r="AAV14" s="0"/>
+      <c r="AAW14" s="0"/>
+      <c r="AAX14" s="0"/>
+      <c r="AAY14" s="0"/>
+      <c r="AAZ14" s="0"/>
+      <c r="ABA14" s="0"/>
+      <c r="ABB14" s="0"/>
+      <c r="ABC14" s="0"/>
+      <c r="ABD14" s="0"/>
+      <c r="ABE14" s="0"/>
+      <c r="ABF14" s="0"/>
+      <c r="ABG14" s="0"/>
+      <c r="ABH14" s="0"/>
+      <c r="ABI14" s="0"/>
+      <c r="ABJ14" s="0"/>
+      <c r="ABK14" s="0"/>
+      <c r="ABL14" s="0"/>
+      <c r="ABM14" s="0"/>
+      <c r="ABN14" s="0"/>
+      <c r="ABO14" s="0"/>
+      <c r="ABP14" s="0"/>
+      <c r="ABQ14" s="0"/>
+      <c r="ABR14" s="0"/>
+      <c r="ABS14" s="0"/>
+      <c r="ABT14" s="0"/>
+      <c r="ABU14" s="0"/>
+      <c r="ABV14" s="0"/>
+      <c r="ABW14" s="0"/>
+      <c r="ABX14" s="0"/>
+      <c r="ABY14" s="0"/>
+      <c r="ABZ14" s="0"/>
+      <c r="ACA14" s="0"/>
+      <c r="ACB14" s="0"/>
+      <c r="ACC14" s="0"/>
+      <c r="ACD14" s="0"/>
+      <c r="ACE14" s="0"/>
+      <c r="ACF14" s="0"/>
+      <c r="ACG14" s="0"/>
+      <c r="ACH14" s="0"/>
+      <c r="ACI14" s="0"/>
+      <c r="ACJ14" s="0"/>
+      <c r="ACK14" s="0"/>
+      <c r="ACL14" s="0"/>
+      <c r="ACM14" s="0"/>
+      <c r="ACN14" s="0"/>
+      <c r="ACO14" s="0"/>
+      <c r="ACP14" s="0"/>
+      <c r="ACQ14" s="0"/>
+      <c r="ACR14" s="0"/>
+      <c r="ACS14" s="0"/>
+      <c r="ACT14" s="0"/>
+      <c r="ACU14" s="0"/>
+      <c r="ACV14" s="0"/>
+      <c r="ACW14" s="0"/>
+      <c r="ACX14" s="0"/>
+      <c r="ACY14" s="0"/>
+      <c r="ACZ14" s="0"/>
+      <c r="ADA14" s="0"/>
+      <c r="ADB14" s="0"/>
+      <c r="ADC14" s="0"/>
+      <c r="ADD14" s="0"/>
+      <c r="ADE14" s="0"/>
+      <c r="ADF14" s="0"/>
+      <c r="ADG14" s="0"/>
+      <c r="ADH14" s="0"/>
+      <c r="ADI14" s="0"/>
+      <c r="ADJ14" s="0"/>
+      <c r="ADK14" s="0"/>
+      <c r="ADL14" s="0"/>
+      <c r="ADM14" s="0"/>
+      <c r="ADN14" s="0"/>
+      <c r="ADO14" s="0"/>
+      <c r="ADP14" s="0"/>
+      <c r="ADQ14" s="0"/>
+      <c r="ADR14" s="0"/>
+      <c r="ADS14" s="0"/>
+      <c r="ADT14" s="0"/>
+      <c r="ADU14" s="0"/>
+      <c r="ADV14" s="0"/>
+      <c r="ADW14" s="0"/>
+      <c r="ADX14" s="0"/>
+      <c r="ADY14" s="0"/>
+      <c r="ADZ14" s="0"/>
+      <c r="AEA14" s="0"/>
+      <c r="AEB14" s="0"/>
+      <c r="AEC14" s="0"/>
+      <c r="AED14" s="0"/>
+      <c r="AEE14" s="0"/>
+      <c r="AEF14" s="0"/>
+      <c r="AEG14" s="0"/>
+      <c r="AEH14" s="0"/>
+      <c r="AEI14" s="0"/>
+      <c r="AEJ14" s="0"/>
+      <c r="AEK14" s="0"/>
+      <c r="AEL14" s="0"/>
+      <c r="AEM14" s="0"/>
+      <c r="AEN14" s="0"/>
+      <c r="AEO14" s="0"/>
+      <c r="AEP14" s="0"/>
+      <c r="AEQ14" s="0"/>
+      <c r="AER14" s="0"/>
+      <c r="AES14" s="0"/>
+      <c r="AET14" s="0"/>
+      <c r="AEU14" s="0"/>
+      <c r="AEV14" s="0"/>
+      <c r="AEW14" s="0"/>
+      <c r="AEX14" s="0"/>
+      <c r="AEY14" s="0"/>
+      <c r="AEZ14" s="0"/>
+      <c r="AFA14" s="0"/>
+      <c r="AFB14" s="0"/>
+      <c r="AFC14" s="0"/>
+      <c r="AFD14" s="0"/>
+      <c r="AFE14" s="0"/>
+      <c r="AFF14" s="0"/>
+      <c r="AFG14" s="0"/>
+      <c r="AFH14" s="0"/>
+      <c r="AFI14" s="0"/>
+      <c r="AFJ14" s="0"/>
+      <c r="AFK14" s="0"/>
+      <c r="AFL14" s="0"/>
+      <c r="AFM14" s="0"/>
+      <c r="AFN14" s="0"/>
+      <c r="AFO14" s="0"/>
+      <c r="AFP14" s="0"/>
+      <c r="AFQ14" s="0"/>
+      <c r="AFR14" s="0"/>
+      <c r="AFS14" s="0"/>
+      <c r="AFT14" s="0"/>
+      <c r="AFU14" s="0"/>
+      <c r="AFV14" s="0"/>
+      <c r="AFW14" s="0"/>
+      <c r="AFX14" s="0"/>
+      <c r="AFY14" s="0"/>
+      <c r="AFZ14" s="0"/>
+      <c r="AGA14" s="0"/>
+      <c r="AGB14" s="0"/>
+      <c r="AGC14" s="0"/>
+      <c r="AGD14" s="0"/>
+      <c r="AGE14" s="0"/>
+      <c r="AGF14" s="0"/>
+      <c r="AGG14" s="0"/>
+      <c r="AGH14" s="0"/>
+      <c r="AGI14" s="0"/>
+      <c r="AGJ14" s="0"/>
+      <c r="AGK14" s="0"/>
+      <c r="AGL14" s="0"/>
+      <c r="AGM14" s="0"/>
+      <c r="AGN14" s="0"/>
+      <c r="AGO14" s="0"/>
+      <c r="AGP14" s="0"/>
+      <c r="AGQ14" s="0"/>
+      <c r="AGR14" s="0"/>
+      <c r="AGS14" s="0"/>
+      <c r="AGT14" s="0"/>
+      <c r="AGU14" s="0"/>
+      <c r="AGV14" s="0"/>
+      <c r="AGW14" s="0"/>
+      <c r="AGX14" s="0"/>
+      <c r="AGY14" s="0"/>
+      <c r="AGZ14" s="0"/>
+      <c r="AHA14" s="0"/>
+      <c r="AHB14" s="0"/>
+      <c r="AHC14" s="0"/>
+      <c r="AHD14" s="0"/>
+      <c r="AHE14" s="0"/>
+      <c r="AHF14" s="0"/>
+      <c r="AHG14" s="0"/>
+      <c r="AHH14" s="0"/>
+      <c r="AHI14" s="0"/>
+      <c r="AHJ14" s="0"/>
+      <c r="AHK14" s="0"/>
+      <c r="AHL14" s="0"/>
+      <c r="AHM14" s="0"/>
+      <c r="AHN14" s="0"/>
+      <c r="AHO14" s="0"/>
+      <c r="AHP14" s="0"/>
+      <c r="AHQ14" s="0"/>
+      <c r="AHR14" s="0"/>
+      <c r="AHS14" s="0"/>
+      <c r="AHT14" s="0"/>
+      <c r="AHU14" s="0"/>
+      <c r="AHV14" s="0"/>
+      <c r="AHW14" s="0"/>
+      <c r="AHX14" s="0"/>
+      <c r="AHY14" s="0"/>
+      <c r="AHZ14" s="0"/>
+      <c r="AIA14" s="0"/>
+      <c r="AIB14" s="0"/>
+      <c r="AIC14" s="0"/>
+      <c r="AID14" s="0"/>
+      <c r="AIE14" s="0"/>
+      <c r="AIF14" s="0"/>
+      <c r="AIG14" s="0"/>
+      <c r="AIH14" s="0"/>
+      <c r="AII14" s="0"/>
+      <c r="AIJ14" s="0"/>
+      <c r="AIK14" s="0"/>
+      <c r="AIL14" s="0"/>
+      <c r="AIM14" s="0"/>
+      <c r="AIN14" s="0"/>
+      <c r="AIO14" s="0"/>
+      <c r="AIP14" s="0"/>
+      <c r="AIQ14" s="0"/>
+      <c r="AIR14" s="0"/>
+      <c r="AIS14" s="0"/>
+      <c r="AIT14" s="0"/>
+      <c r="AIU14" s="0"/>
+      <c r="AIV14" s="0"/>
+      <c r="AIW14" s="0"/>
+      <c r="AIX14" s="0"/>
+      <c r="AIY14" s="0"/>
+      <c r="AIZ14" s="0"/>
+      <c r="AJA14" s="0"/>
+      <c r="AJB14" s="0"/>
+      <c r="AJC14" s="0"/>
+      <c r="AJD14" s="0"/>
+      <c r="AJE14" s="0"/>
+      <c r="AJF14" s="0"/>
+      <c r="AJG14" s="0"/>
+      <c r="AJH14" s="0"/>
+      <c r="AJI14" s="0"/>
+      <c r="AJJ14" s="0"/>
+      <c r="AJK14" s="0"/>
+      <c r="AJL14" s="0"/>
+      <c r="AJM14" s="0"/>
+      <c r="AJN14" s="0"/>
+      <c r="AJO14" s="0"/>
+      <c r="AJP14" s="0"/>
+      <c r="AJQ14" s="0"/>
+      <c r="AJR14" s="0"/>
+      <c r="AJS14" s="0"/>
+      <c r="AJT14" s="0"/>
+      <c r="AJU14" s="0"/>
+      <c r="AJV14" s="0"/>
+      <c r="AJW14" s="0"/>
+      <c r="AJX14" s="0"/>
+      <c r="AJY14" s="0"/>
+      <c r="AJZ14" s="0"/>
+      <c r="AKA14" s="0"/>
+      <c r="AKB14" s="0"/>
+      <c r="AKC14" s="0"/>
+      <c r="AKD14" s="0"/>
+      <c r="AKE14" s="0"/>
+      <c r="AKF14" s="0"/>
+      <c r="AKG14" s="0"/>
+      <c r="AKH14" s="0"/>
+      <c r="AKI14" s="0"/>
+      <c r="AKJ14" s="0"/>
+      <c r="AKK14" s="0"/>
+      <c r="AKL14" s="0"/>
+      <c r="AKM14" s="0"/>
+      <c r="AKN14" s="0"/>
+      <c r="AKO14" s="0"/>
+      <c r="AKP14" s="0"/>
+      <c r="AKQ14" s="0"/>
+      <c r="AKR14" s="0"/>
+      <c r="AKS14" s="0"/>
+      <c r="AKT14" s="0"/>
+      <c r="AKU14" s="0"/>
+      <c r="AKV14" s="0"/>
+      <c r="AKW14" s="0"/>
+      <c r="AKX14" s="0"/>
+      <c r="AKY14" s="0"/>
+      <c r="AKZ14" s="0"/>
+      <c r="ALA14" s="0"/>
+      <c r="ALB14" s="0"/>
+      <c r="ALC14" s="0"/>
+      <c r="ALD14" s="0"/>
+      <c r="ALE14" s="0"/>
+      <c r="ALF14" s="0"/>
+      <c r="ALG14" s="0"/>
+      <c r="ALH14" s="0"/>
+      <c r="ALI14" s="0"/>
+      <c r="ALJ14" s="0"/>
+      <c r="ALK14" s="0"/>
+      <c r="ALL14" s="0"/>
+      <c r="ALM14" s="0"/>
+      <c r="ALN14" s="0"/>
+      <c r="ALO14" s="0"/>
+      <c r="ALP14" s="0"/>
+      <c r="ALQ14" s="0"/>
+      <c r="ALR14" s="0"/>
+      <c r="ALS14" s="0"/>
+      <c r="ALT14" s="0"/>
+      <c r="ALU14" s="0"/>
+      <c r="ALV14" s="0"/>
+      <c r="ALW14" s="0"/>
+      <c r="ALX14" s="0"/>
+      <c r="ALY14" s="0"/>
+      <c r="ALZ14" s="0"/>
+      <c r="AMA14" s="0"/>
+      <c r="AMB14" s="0"/>
+      <c r="AMC14" s="0"/>
+      <c r="AMD14" s="0"/>
+      <c r="AME14" s="0"/>
+      <c r="AMF14" s="0"/>
+      <c r="AMG14" s="0"/>
+      <c r="AMH14" s="0"/>
+      <c r="AMI14" s="0"/>
+      <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4216,6 +5322,7 @@
     <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4232,10 +5339,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1006"/>
+  <dimension ref="A1:G1007"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4256,22 +5363,22 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>71</v>
+        <v>80</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4279,27 +5386,27 @@
         <v>26</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>79</v>
+      <c r="B3" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4307,85 +5414,85 @@
         <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>82</v>
+      <c r="B5" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>84</v>
+      <c r="B6" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="13"/>
+        <v>96</v>
+      </c>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>87</v>
+      <c r="B7" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="13"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>89</v>
+      <c r="B8" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>92</v>
+      <c r="B9" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4393,33 +5500,33 @@
         <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="14" t="s">
+      <c r="B11" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>35</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4427,168 +5534,174 @@
         <v>29</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E12" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>32</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>101</v>
+      <c r="B13" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>105</v>
+      <c r="B14" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>106</v>
+      <c r="B15" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>107</v>
+      <c r="B16" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>109</v>
+      <c r="B17" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>111</v>
+      <c r="B18" s="14" t="s">
+        <v>119</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>47</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>112</v>
+      <c r="B19" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>50</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>113</v>
+      <c r="B20" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>38</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>115</v>
+      <c r="B21" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>118</v>
+      <c r="A22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4596,69 +5709,65 @@
         <v>47</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>118</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>78</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="D26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>126</v>
+        <v>115</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4666,13 +5775,13 @@
         <v>38</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4680,17 +5789,13 @@
         <v>38</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D29" s="0"/>
-      <c r="E29" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>124</v>
+        <v>136</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4698,27 +5803,35 @@
         <v>38</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C30" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="0"/>
+      <c r="E30" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>133</v>
+      <c r="G30" s="9" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>78</v>
+        <v>139</v>
+      </c>
+      <c r="D31" s="0"/>
+      <c r="E31" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4726,13 +5839,13 @@
         <v>41</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4740,31 +5853,31 @@
         <v>41</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>121</v>
+        <v>144</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>124</v>
+        <v>62</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4772,30 +5885,34 @@
         <v>44</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>139</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="D35" s="0"/>
       <c r="E35" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>86</v>
+      <c r="F36" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4803,16 +5920,33 @@
         <v>56</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>144</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="0"/>
+      <c r="E38" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5781,10 +6915,8 @@
     <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C14" r:id="rId1" display="https://en.wikipedia.org/wiki/{country_name}"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5817,13 +6949,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Segunda versión del mapeo mediante r2rml
- falta por cuadradar el tipo de condición
- salida generada añadida
- faltan por añadir los skos
</commit_message>
<xml_diff>
--- a/data_mappeator/InputPhotocalysisMapping.xlsx
+++ b/data_mappeator/InputPhotocalysisMapping.xlsx
@@ -218,7 +218,7 @@
     <t xml:space="preserve">qudt:Unit</t>
   </si>
   <si>
-    <t xml:space="preserve">unit:{UNIT}</t>
+    <t xml:space="preserve">http://qudt.org/vocab/unit/{UNIT}</t>
   </si>
   <si>
     <t xml:space="preserve">MaterialTransformationRole</t>
@@ -227,7 +227,7 @@
     <t xml:space="preserve">phcat:MaterialTransformationRole</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.example.com/material_transformation_role/{Role}</t>
+    <t xml:space="preserve">http://data.example.com/material_transformation_role/{ROLE}</t>
   </si>
   <si>
     <t xml:space="preserve">Feature</t>
@@ -1953,7 +1953,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3127,6 +3127,8 @@
     <hyperlink ref="C9" r:id="rId5" display="http://data.example.com/eg/{ID}"/>
     <hyperlink ref="C10" r:id="rId6" display="http://data.example.com/bet/{ID}"/>
     <hyperlink ref="C13" r:id="rId7" display="https://en.wikipedia.org/wiki/"/>
+    <hyperlink ref="C14" r:id="rId8" display="http://qudt.org/vocab/unit/"/>
+    <hyperlink ref="C15" r:id="rId9" display="http://data.example.com/material_transformation_role/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3146,7 +3148,7 @@
   <dimension ref="A1:AMJ993"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4342,7 +4344,7 @@
         <v>70</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5342,7 +5344,7 @@
   <dimension ref="A1:G1007"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Añadido al mapeo las clases de condiciones exactas
</commit_message>
<xml_diff>
--- a/data_mappeator/InputPhotocalysisMapping.xlsx
+++ b/data_mappeator/InputPhotocalysisMapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" state="visible" r:id="rId2"/>
@@ -1952,8 +1952,8 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3147,8 +3147,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ993"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Corregida extracción de datos
- relación de papers con procesos por columna No_de_ref en lugar de ID
</commit_message>
<xml_diff>
--- a/data_mappeator/InputPhotocalysisMapping.xlsx
+++ b/data_mappeator/InputPhotocalysisMapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" state="visible" r:id="rId2"/>
@@ -540,7 +540,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -591,12 +591,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -657,7 +651,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -698,15 +692,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -718,11 +708,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -809,7 +795,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.67"/>
@@ -1952,11 +1938,11 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.57"/>
@@ -2006,7 +1992,7 @@
       <c r="B4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2134,7 +2120,7 @@
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3120,15 +3106,15 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="http://data.example.com/author/"/>
+    <hyperlink ref="C4" r:id="rId1" display="http://data.example.com/author/{NAME}-{ID}"/>
     <hyperlink ref="C6" r:id="rId2" display="http://data.example.com/input/{ID}"/>
     <hyperlink ref="C7" r:id="rId3" display="http://data.example.com/condition/{ID}"/>
     <hyperlink ref="C8" r:id="rId4" display="http://data.example.com/output/{ID}"/>
     <hyperlink ref="C9" r:id="rId5" display="http://data.example.com/eg/{ID}"/>
     <hyperlink ref="C10" r:id="rId6" display="http://data.example.com/bet/{ID}"/>
-    <hyperlink ref="C13" r:id="rId7" display="https://en.wikipedia.org/wiki/"/>
-    <hyperlink ref="C14" r:id="rId8" display="http://qudt.org/vocab/unit/"/>
-    <hyperlink ref="C15" r:id="rId9" display="http://data.example.com/material_transformation_role/"/>
+    <hyperlink ref="C13" r:id="rId7" display="https://en.wikipedia.org/wiki/{COUNTRY_NAME}"/>
+    <hyperlink ref="C14" r:id="rId8" display="http://qudt.org/vocab/unit/{UNIT}"/>
+    <hyperlink ref="C15" r:id="rId9" display="http://data.example.com/material_transformation_role/{ROLE}"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3162,13 +3148,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5343,8 +5329,8 @@
   </sheetPr>
   <dimension ref="A1:G1007"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5367,7 +5353,7 @@
       <c r="B1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -5401,7 +5387,7 @@
       <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -5429,7 +5415,7 @@
       <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -5443,7 +5429,7 @@
       <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>94</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -5452,13 +5438,13 @@
       <c r="D6" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>97</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -5467,13 +5453,13 @@
       <c r="D7" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>99</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -5487,7 +5473,7 @@
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>102</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -5518,14 +5504,14 @@
       <c r="A11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>35</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>108</v>
@@ -5538,7 +5524,7 @@
       <c r="B12" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>32</v>
       </c>
       <c r="F12" s="9" t="s">
@@ -5552,7 +5538,7 @@
       <c r="A13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>111</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -5563,7 +5549,7 @@
       <c r="A14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>112</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -5577,27 +5563,27 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>114</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="9" t="s">
         <v>108</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>115</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -5608,10 +5594,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>117</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -5622,10 +5608,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>119</v>
       </c>
       <c r="E18" s="9" t="s">
@@ -5639,10 +5625,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>120</v>
       </c>
       <c r="E19" s="9" t="s">
@@ -5656,10 +5642,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>121</v>
       </c>
       <c r="E20" s="9" t="s">
@@ -5673,10 +5659,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>123</v>
       </c>
       <c r="E21" s="9" t="s">
@@ -5690,10 +5676,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>124</v>
       </c>
       <c r="E22" s="9" t="s">
@@ -5875,7 +5861,7 @@
       <c r="E34" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="9" t="s">
         <v>145</v>
       </c>
       <c r="G34" s="9" t="s">
@@ -5942,7 +5928,7 @@
       <c r="E38" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="9" t="s">
         <v>145</v>
       </c>
       <c r="G38" s="9" t="s">
@@ -6940,7 +6926,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.67"/>
@@ -6950,13 +6936,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizado mapeo con conceptos SKOS
</commit_message>
<xml_diff>
--- a/data_mappeator/InputPhotocalysisMapping.xlsx
+++ b/data_mappeator/InputPhotocalysisMapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="160">
   <si>
     <t xml:space="preserve">Prefix</t>
   </si>
@@ -437,7 +437,7 @@
     <t xml:space="preserve">phcat:operationMode</t>
   </si>
   <si>
-    <t xml:space="preserve">{OPERATION_MODE}</t>
+    <t xml:space="preserve">http://vocab.example.com/condition/operationMode/{OPERATION_MODE}</t>
   </si>
   <si>
     <t xml:space="preserve">phcat:hasReactionEg</t>
@@ -506,10 +506,40 @@
     <t xml:space="preserve">{ROLE}</t>
   </si>
   <si>
-    <t xml:space="preserve">phcat:conditionType</t>
+    <t xml:space="preserve">phcat:conditionTypeAsText</t>
   </si>
   <si>
     <t xml:space="preserve">{TYPE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:reactorType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{REACTOR_TYPE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:setUpType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{SET_UP_TYPE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:lampType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{LAMP_TYPE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:reactionMediumType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://vocab.example.com/condition/reactionMediumType/{REACTION_MEDIUM_TYPE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:lightSourceType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://vocab.example.com/condition/lightSourceType/{LIGHT_SOURCE_TYPE}</t>
   </si>
   <si>
     <t xml:space="preserve">qudt:value</t>
@@ -540,7 +570,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -591,12 +621,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -657,7 +681,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -698,15 +722,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -718,11 +738,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -799,17 +815,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="E37:E38 A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.67"/>
@@ -1946,17 +1962,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="E37:E38 C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.57"/>
@@ -2006,7 +2022,7 @@
       <c r="B4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2134,7 +2150,7 @@
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3120,15 +3136,15 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="http://data.example.com/author/"/>
+    <hyperlink ref="C4" r:id="rId1" display="http://data.example.com/author/{NAME}-{ID}"/>
     <hyperlink ref="C6" r:id="rId2" display="http://data.example.com/input/{ID}"/>
     <hyperlink ref="C7" r:id="rId3" display="http://data.example.com/condition/{ID}"/>
     <hyperlink ref="C8" r:id="rId4" display="http://data.example.com/output/{ID}"/>
     <hyperlink ref="C9" r:id="rId5" display="http://data.example.com/eg/{ID}"/>
     <hyperlink ref="C10" r:id="rId6" display="http://data.example.com/bet/{ID}"/>
-    <hyperlink ref="C13" r:id="rId7" display="https://en.wikipedia.org/wiki/"/>
-    <hyperlink ref="C14" r:id="rId8" display="http://qudt.org/vocab/unit/"/>
-    <hyperlink ref="C15" r:id="rId9" display="http://data.example.com/material_transformation_role/"/>
+    <hyperlink ref="C13" r:id="rId7" display="https://en.wikipedia.org/wiki/{COUNTRY_NAME}"/>
+    <hyperlink ref="C14" r:id="rId8" display="http://qudt.org/vocab/unit/{UNIT}"/>
+    <hyperlink ref="C15" r:id="rId9" display="http://data.example.com/material_transformation_role/{ROLE}"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3141,34 +3157,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ993"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="1" sqref="E37:E38 A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="28.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="11.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="30.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="9" width="10.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="9" width="8.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="9" width="11.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="27" style="9" width="11.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5337,27 +5353,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1007"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E37:E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="28.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="36.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="40.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="72.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="9" width="30.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="28.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="11.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="30.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="9" width="8.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="9" width="11.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="27" style="9" width="11.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5367,7 +5383,7 @@
       <c r="B1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -5401,7 +5417,7 @@
       <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -5429,7 +5445,7 @@
       <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -5443,7 +5459,7 @@
       <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>94</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -5452,13 +5468,13 @@
       <c r="D6" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>97</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -5467,13 +5483,13 @@
       <c r="D7" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>99</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -5487,7 +5503,7 @@
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>102</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -5518,10 +5534,10 @@
       <c r="A11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>35</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -5538,7 +5554,7 @@
       <c r="B12" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>32</v>
       </c>
       <c r="F12" s="9" t="s">
@@ -5552,7 +5568,7 @@
       <c r="A13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>111</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -5563,7 +5579,7 @@
       <c r="A14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>112</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -5577,16 +5593,16 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>114</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="9" t="s">
         <v>108</v>
       </c>
       <c r="G15" s="9" t="s">
@@ -5594,10 +5610,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>115</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -5608,24 +5624,21 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>117</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>119</v>
       </c>
       <c r="E18" s="9" t="s">
@@ -5639,10 +5652,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>120</v>
       </c>
       <c r="E19" s="9" t="s">
@@ -5656,10 +5669,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>121</v>
       </c>
       <c r="E20" s="9" t="s">
@@ -5673,10 +5686,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>123</v>
       </c>
       <c r="E21" s="9" t="s">
@@ -5690,10 +5703,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>124</v>
       </c>
       <c r="E22" s="9" t="s">
@@ -5869,91 +5882,150 @@
         <v>41</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D34" s="0"/>
-      <c r="E34" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="C34" s="9" t="s">
         <v>146</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="0"/>
-      <c r="E35" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>132</v>
+        <v>147</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>106</v>
+        <v>149</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="0"/>
+      <c r="E39" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D40" s="0"/>
+      <c r="E40" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="F41" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D38" s="0"/>
-      <c r="E38" s="9" t="s">
+      <c r="D43" s="0"/>
+      <c r="E43" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F38" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="F43" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6918,7 +6990,18 @@
     <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1008" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1009" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1010" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1011" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1012" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C17" r:id="rId1" display="http://vocab.example.com/condition/operationMode/"/>
+    <hyperlink ref="C36" r:id="rId2" display="http://vocab.example.com/condition/reactionMediumType/"/>
+    <hyperlink ref="C37" r:id="rId3" display="http://vocab.example.com/condition/lightSourceType/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6930,17 +7013,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E37:E38 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.67"/>
@@ -6950,13 +7033,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B1" s="16" t="s">
+      <c r="A1" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corregido excel mapeo tras merge
- añadida nuevamente información sobre SKOS a mapeo
- tras el merge la info de master se perdio. Se ha añadido nuevamente
</commit_message>
<xml_diff>
--- a/data_mappeator/InputPhotocalysisMapping.xlsx
+++ b/data_mappeator/InputPhotocalysisMapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="160">
   <si>
     <t xml:space="preserve">Prefix</t>
   </si>
@@ -437,7 +437,7 @@
     <t xml:space="preserve">phcat:operationMode</t>
   </si>
   <si>
-    <t xml:space="preserve">{OPERATION_MODE}</t>
+    <t xml:space="preserve">http://vocab.example.com/condition/operationMode/{OPERATION_MODE}</t>
   </si>
   <si>
     <t xml:space="preserve">phcat:hasReactionEg</t>
@@ -506,10 +506,40 @@
     <t xml:space="preserve">{ROLE}</t>
   </si>
   <si>
-    <t xml:space="preserve">phcat:conditionType</t>
+    <t xml:space="preserve">phcat:conditionTypeAsText</t>
   </si>
   <si>
     <t xml:space="preserve">{TYPE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:reactorType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{REACTOR_TYPE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:setUpType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{SET_UP_TYPE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:lampType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{LAMP_TYPE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:reactionMediumType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://vocab.example.com/condition/reactionMediumType/{REACTION_MEDIUM_TYPE}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:lightSourceType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://vocab.example.com/condition/lightSourceType/{LIGHT_SOURCE_TYPE}</t>
   </si>
   <si>
     <t xml:space="preserve">qudt:value</t>
@@ -795,7 +825,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.67"/>
@@ -1942,7 +1972,7 @@
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.57"/>
@@ -5327,17 +5357,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1007"/>
+  <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="28.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="36.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="40.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="72.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="9" width="30.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="28.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="11.8"/>
@@ -5603,9 +5633,6 @@
       <c r="C17" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
@@ -5855,91 +5882,150 @@
         <v>41</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D34" s="0"/>
-      <c r="E34" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="C34" s="9" t="s">
         <v>146</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="0"/>
-      <c r="E35" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>132</v>
+        <v>147</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>106</v>
+        <v>149</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="0"/>
+      <c r="E39" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D40" s="0"/>
+      <c r="E40" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="F41" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D38" s="0"/>
-      <c r="E38" s="9" t="s">
+      <c r="D43" s="0"/>
+      <c r="E43" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F38" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="F43" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6904,7 +6990,17 @@
     <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1008" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1009" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1010" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1011" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1012" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C17" r:id="rId1" display="http://vocab.example.com/condition/operationMode/{OPERATION_MODE}"/>
+    <hyperlink ref="C36" r:id="rId2" display="http://vocab.example.com/condition/reactionMediumType/{REACTION_MEDIUM_TYPE}"/>
+    <hyperlink ref="C37" r:id="rId3" display="http://vocab.example.com/condition/lightSourceType/{LIGHT_SOURCE_TYPE}"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6926,7 +7022,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.67"/>
@@ -6937,7 +7033,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Corrección URIs para roles de transformación
</commit_message>
<xml_diff>
--- a/data_mappeator/InputPhotocalysisMapping.xlsx
+++ b/data_mappeator/InputPhotocalysisMapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" state="visible" r:id="rId2"/>
@@ -227,7 +227,7 @@
     <t xml:space="preserve">phcat:MaterialTransformationRole</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.example.com/material_transformation_role/{ROLE}</t>
+    <t xml:space="preserve">http://data.example.com/{ROLE}</t>
   </si>
   <si>
     <t xml:space="preserve">Feature</t>
@@ -815,7 +815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -825,7 +825,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.67"/>
@@ -1952,8 +1952,8 @@
     <hyperlink ref="B8" r:id="rId7" display="https://schema.org/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1962,17 +1962,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.57"/>
@@ -3144,11 +3144,10 @@
     <hyperlink ref="C10" r:id="rId6" display="http://data.example.com/bet/{ID}"/>
     <hyperlink ref="C13" r:id="rId7" display="https://en.wikipedia.org/wiki/{COUNTRY_NAME}"/>
     <hyperlink ref="C14" r:id="rId8" display="http://qudt.org/vocab/unit/{UNIT}"/>
-    <hyperlink ref="C15" r:id="rId9" display="http://data.example.com/material_transformation_role/{ROLE}"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3157,7 +3156,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3174,7 +3173,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="30.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="9" width="10.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="9" width="8.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="27" style="9" width="11.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="9" width="11.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5343,8 +5342,8 @@
     <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5353,14 +5352,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5373,7 +5372,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="11.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="30.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="9" width="8.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="27" style="9" width="11.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="9" width="11.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7002,8 +7001,8 @@
     <hyperlink ref="C37" r:id="rId3" display="http://vocab.example.com/condition/lightSourceType/{LIGHT_SOURCE_TYPE}"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7012,7 +7011,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -7022,7 +7021,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.67"/>
@@ -8044,7 +8043,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>